<commit_message>
feat(mpe, utils): add function delete_other_columns using the function of utils columns_from_strings
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_colcongruent.xlsx
+++ b/fichiers_xls/test_colcongruent.xlsx
@@ -349,8 +349,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="954" max="1023"/>
-    <col width="11.53" customWidth="1" style="2" min="16384" max="16384"/>
+    <col width="11.52" customWidth="1" style="2" min="953" max="1022"/>
+    <col width="11.53" customWidth="1" style="2" min="16383" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" s="3">
@@ -384,7 +384,7 @@
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>congruent1_.jpg</t>
+          <t>congruent1_o.jpg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -403,7 +403,7 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>incongruent1_.jpg</t>
+          <t>incongruent1_n.jpg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -422,7 +422,7 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>congruent2_.jpg</t>
+          <t>congruent2_o.jpg</t>
         </is>
       </c>
       <c r="E4" s="2" t="n"/>
@@ -436,7 +436,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>congruent3_.jpg</t>
+          <t>congruent3_n.jpg</t>
         </is>
       </c>
     </row>
@@ -448,7 +448,7 @@
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>congruent5_.jpg</t>
+          <t>congruent5_o.jpg</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -465,7 +465,7 @@
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>d1_.jpg</t>
+          <t>d1_o.jpg</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>congruent1_.jpg</t>
+          <t>congruent1_o.jpg</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>neutre12_.jpg</t>
+          <t>neutre12_n.jpg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">

</xml_diff>

<commit_message>
factor(module_pour_excel): write and tests multiple methods with the descriptor act_on_columns
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_colcongruent.xlsx
+++ b/fichiers_xls/test_colcongruent.xlsx
@@ -341,7 +341,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
@@ -369,7 +369,7 @@
           <t>Multiplisme</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Colonne de(s) maximum(s)</t>
         </is>
@@ -392,7 +392,12 @@
           <t>prime_congruent</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>prime_congruent</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="n"/>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="3">
       <c r="A3" s="2" t="n"/>
@@ -411,7 +416,12 @@
           <t>probe_incongruent</t>
         </is>
       </c>
-      <c r="E3" s="2" t="n"/>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>probe_incongruent</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="n"/>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="3">
       <c r="A4" s="2" t="n"/>
@@ -425,7 +435,7 @@
           <t>congruent2_o.jpg</t>
         </is>
       </c>
-      <c r="E4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="3">
       <c r="A5" s="2" t="n"/>
@@ -456,6 +466,11 @@
           <t>probe_congruent</t>
         </is>
       </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>probe_congruent</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="3">
       <c r="B7" s="2" t="inlineStr">
@@ -493,6 +508,11 @@
         </is>
       </c>
       <c r="D9" t="inlineStr">
+        <is>
+          <t>prime_neutre</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>prime_neutre</t>
         </is>

</xml_diff>

<commit_message>
feat(module_pour_excel, xlspython): change the aim of colcongruent
</commit_message>
<xml_diff>
--- a/fichiers_xls/test_colcongruent.xlsx
+++ b/fichiers_xls/test_colcongruent.xlsx
@@ -69,7 +69,10 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -344,184 +347,247 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="953" max="1022"/>
-    <col width="11.53" customWidth="1" style="2" min="16383" max="16384"/>
+    <col width="11.52" customWidth="1" style="3" min="951" max="1020"/>
+    <col width="11.53" customWidth="1" style="3" min="16381" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Evaluatisme</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Absolutisme</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Multiplisme</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Multiplisme</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Colonne de(s) maximum(s)</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="3">
-      <c r="A2" s="2" t="n"/>
-      <c r="B2" s="2" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="4">
+      <c r="A2" s="3" t="n"/>
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>prime</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>congruent1_o.jpg</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>congruent1_o.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>prime_congruent</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>prime_congruent</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="n"/>
-    </row>
-    <row r="3" ht="12.75" customHeight="1" s="3">
-      <c r="A3" s="2" t="n"/>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="4">
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>probe</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>incongruent1_n.jpg</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>incongruent1_n.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>probe_incongruent</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>probe_incongruent</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n"/>
-    </row>
-    <row r="4" ht="12.75" customHeight="1" s="3">
-      <c r="A4" s="2" t="n"/>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="4">
+      <c r="A4" s="3" t="n"/>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>qfqfq</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>congruent2_o.jpg</t>
         </is>
       </c>
-      <c r="F4" s="2" t="n"/>
-    </row>
-    <row r="5" ht="12.75" customHeight="1" s="3">
-      <c r="A5" s="2" t="n"/>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>congruent2_o.jpg</t>
+        </is>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="4">
+      <c r="A5" s="3" t="n"/>
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>qvfqf</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>congruent3_n.jpg</t>
         </is>
       </c>
-    </row>
-    <row r="6" ht="12.75" customHeight="1" s="3">
-      <c r="B6" s="2" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>congruent3_n.jpg</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="4">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>probe</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>congruent5_o.jpg</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>congruent5_o.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>probe_congruent</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>probe_congruent</t>
-        </is>
-      </c>
-    </row>
-    <row r="7" ht="12.75" customHeight="1" s="3">
-      <c r="B7" s="2" t="inlineStr">
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="4">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>pqfqf</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>d1_o.jpg</t>
         </is>
       </c>
-    </row>
-    <row r="8" ht="12.75" customHeight="1" s="3">
-      <c r="B8" s="2" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>d1_o.jpg</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>af</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="4">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>Prime</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>congruent1_o.jpg</t>
         </is>
       </c>
-    </row>
-    <row r="9" ht="12.75" customHeight="1" s="3">
-      <c r="B9" s="2" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>congruent1_o.jpg</t>
+        </is>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="4">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>prime</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>neutre12_n.jpg</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>neutre12_n.jpg</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>prime_neutre</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>prime_neutre</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="12.75" customHeight="1" s="3">
-      <c r="A10" s="2" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" s="4">
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="3" t="n"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>

</xml_diff>